<commit_message>
fixed corrupted population data
</commit_message>
<xml_diff>
--- a/midterm/mock_exam/data/EXIOBASE_PopulationGDP_1995_2019.xlsx
+++ b/midterm/mock_exam/data/EXIOBASE_PopulationGDP_1995_2019.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leidenuniv1-my.sharepoint.com/personal/donatif_vuw_leidenuniv_nl/Documents/1_CML/2_teaching/EEIO/advanced_EEIO_course_notebooks/midterm/exam_mockup/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leidenuniv1-my.sharepoint.com/personal/donatif_vuw_leidenuniv_nl/Documents/1_CML/2_teaching/EEIO/advanced_EEIO_course_sv/midterm/mock_exam/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{C3DA41E7-5A46-402B-96DD-F574E69A010A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA59EC2C-1AB5-45CD-B58E-7789419491E6}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{C3DA41E7-5A46-402B-96DD-F574E69A010A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79F70DDD-941A-4A4A-B339-E0D6FC19944A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{EA179B0C-DA68-4278-82EF-B259CC14BBCB}"/>
+    <workbookView xWindow="-135" yWindow="315" windowWidth="29070" windowHeight="16020" xr2:uid="{EA179B0C-DA68-4278-82EF-B259CC14BBCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Population" sheetId="1" r:id="rId1"/>
@@ -903,13 +903,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77046716-45E2-41A6-9BAE-3175BD5ED5A2}">
   <dimension ref="A1:AB50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:AB50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>147</v>
       </c>
@@ -986,7 +986,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -1063,16 +1063,16 @@
         <v>8473786</v>
       </c>
       <c r="Z2">
-        <v>11195138</v>
+        <v>8473786</v>
       </c>
       <c r="AA2">
-        <v>11195138</v>
+        <v>8473786</v>
       </c>
       <c r="AB2">
-        <v>11195138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+        <v>8473786</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -1149,16 +1149,16 @@
         <v>11195138</v>
       </c>
       <c r="Z3">
-        <v>6978840.4811911499</v>
+        <v>11195138</v>
       </c>
       <c r="AA3">
-        <v>6909052.0763792396</v>
+        <v>11195138</v>
       </c>
       <c r="AB3">
-        <v>6839961.5556154503</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+        <v>11195138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -1235,16 +1235,16 @@
         <v>7049333.8193849996</v>
       </c>
       <c r="Z4">
-        <v>1187501.9156756599</v>
+        <v>6978840.4811911499</v>
       </c>
       <c r="AA4">
-        <v>1199376.93483242</v>
+        <v>6909052.0763792396</v>
       </c>
       <c r="AB4">
-        <v>1211370.7041807401</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+        <v>6839961.5556154503</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -1321,16 +1321,16 @@
         <v>1175744.4709660001</v>
       </c>
       <c r="Z5">
-        <v>10521468</v>
+        <v>1187501.9156756599</v>
       </c>
       <c r="AA5">
-        <v>10521468</v>
+        <v>1199376.93483242</v>
       </c>
       <c r="AB5">
-        <v>10521468</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+        <v>1211370.7041807401</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -1407,16 +1407,16 @@
         <v>10521468</v>
       </c>
       <c r="Z6">
-        <v>80621788</v>
+        <v>10521468</v>
       </c>
       <c r="AA6">
-        <v>80621788</v>
+        <v>10521468</v>
       </c>
       <c r="AB6">
-        <v>80621788</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+        <v>10521468</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -1493,16 +1493,16 @@
         <v>80621788</v>
       </c>
       <c r="Z7">
-        <v>5613706</v>
+        <v>80621788</v>
       </c>
       <c r="AA7">
-        <v>5613706</v>
+        <v>80621788</v>
       </c>
       <c r="AB7">
-        <v>5613706</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+        <v>80621788</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -1579,16 +1579,16 @@
         <v>5613706</v>
       </c>
       <c r="Z8">
-        <v>1324612</v>
+        <v>5613706</v>
       </c>
       <c r="AA8">
-        <v>1324612</v>
+        <v>5613706</v>
       </c>
       <c r="AB8">
-        <v>1324612</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+        <v>5613706</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -1665,16 +1665,16 @@
         <v>1324612</v>
       </c>
       <c r="Z9">
-        <v>46647421</v>
+        <v>1324612</v>
       </c>
       <c r="AA9">
-        <v>46647421</v>
+        <v>1324612</v>
       </c>
       <c r="AB9">
-        <v>46647421</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+        <v>1324612</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -1751,16 +1751,16 @@
         <v>46647421</v>
       </c>
       <c r="Z10">
-        <v>5439407</v>
+        <v>46647421</v>
       </c>
       <c r="AA10">
-        <v>5439407</v>
+        <v>46647421</v>
       </c>
       <c r="AB10">
-        <v>5439407</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+        <v>46647421</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>107</v>
       </c>
@@ -1837,16 +1837,16 @@
         <v>5439407</v>
       </c>
       <c r="Z11">
-        <v>66028467</v>
+        <v>5439407</v>
       </c>
       <c r="AA11">
-        <v>66028467</v>
+        <v>5439407</v>
       </c>
       <c r="AB11">
-        <v>66028467</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+        <v>5439407</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -1923,16 +1923,16 @@
         <v>66028467</v>
       </c>
       <c r="Z12">
-        <v>11032328</v>
+        <v>66028467</v>
       </c>
       <c r="AA12">
-        <v>11032328</v>
+        <v>66028467</v>
       </c>
       <c r="AB12">
-        <v>11032328</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+        <v>66028467</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -2009,16 +2009,16 @@
         <v>11032328</v>
       </c>
       <c r="Z13">
-        <v>4252700</v>
+        <v>11032328</v>
       </c>
       <c r="AA13">
-        <v>4252700</v>
+        <v>11032328</v>
       </c>
       <c r="AB13">
-        <v>4252700</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+        <v>11032328</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>110</v>
       </c>
@@ -2095,16 +2095,16 @@
         <v>4252700</v>
       </c>
       <c r="Z14">
-        <v>9897247</v>
+        <v>4252700</v>
       </c>
       <c r="AA14">
-        <v>9897247</v>
+        <v>4252700</v>
       </c>
       <c r="AB14">
-        <v>9897247</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+        <v>4252700</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>111</v>
       </c>
@@ -2181,16 +2181,16 @@
         <v>9897247</v>
       </c>
       <c r="Z15">
-        <v>4781867.8356768098</v>
+        <v>9897247</v>
       </c>
       <c r="AA15">
-        <v>4829686.5140335802</v>
+        <v>9897247</v>
       </c>
       <c r="AB15">
-        <v>4877983.3791739102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+        <v>9897247</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>112</v>
       </c>
@@ -2267,16 +2267,16 @@
         <v>4734522.6095810002</v>
       </c>
       <c r="Z16">
-        <v>59831093</v>
+        <v>4781867.8356768098</v>
       </c>
       <c r="AA16">
-        <v>59831093</v>
+        <v>4829686.5140335802</v>
       </c>
       <c r="AB16">
-        <v>59831093</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+        <v>4877983.3791739102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>113</v>
       </c>
@@ -2353,16 +2353,16 @@
         <v>59831093</v>
       </c>
       <c r="Z17">
-        <v>2956121</v>
+        <v>59831093</v>
       </c>
       <c r="AA17">
-        <v>2956121</v>
+        <v>59831093</v>
       </c>
       <c r="AB17">
-        <v>2956121</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+        <v>59831093</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>114</v>
       </c>
@@ -2439,16 +2439,16 @@
         <v>2956121</v>
       </c>
       <c r="Z18">
-        <v>565258.17944002</v>
+        <v>2956121</v>
       </c>
       <c r="AA18">
-        <v>570910.76123442</v>
+        <v>2956121</v>
       </c>
       <c r="AB18">
-        <v>576619.86884676397</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+        <v>2956121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>115</v>
       </c>
@@ -2525,16 +2525,16 @@
         <v>559661.56380200002</v>
       </c>
       <c r="Z19">
-        <v>2013385</v>
+        <v>565258.17944002</v>
       </c>
       <c r="AA19">
-        <v>2013385</v>
+        <v>570910.76123442</v>
       </c>
       <c r="AB19">
-        <v>2013385</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+        <v>576619.86884676397</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>116</v>
       </c>
@@ -2611,16 +2611,16 @@
         <v>2013385</v>
       </c>
       <c r="Z20">
-        <v>423282</v>
+        <v>2013385</v>
       </c>
       <c r="AA20">
-        <v>423282</v>
+        <v>2013385</v>
       </c>
       <c r="AB20">
-        <v>423282</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+        <v>2013385</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -2697,16 +2697,16 @@
         <v>423282</v>
       </c>
       <c r="Z21">
-        <v>16804224</v>
+        <v>423282</v>
       </c>
       <c r="AA21">
-        <v>16804224</v>
+        <v>423282</v>
       </c>
       <c r="AB21">
-        <v>16804224</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+        <v>423282</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>118</v>
       </c>
@@ -2783,16 +2783,16 @@
         <v>16804224</v>
       </c>
       <c r="Z22">
-        <v>38530725</v>
+        <v>16804224</v>
       </c>
       <c r="AA22">
-        <v>38530725</v>
+        <v>16804224</v>
       </c>
       <c r="AB22">
-        <v>38530725</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+        <v>16804224</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>119</v>
       </c>
@@ -2869,16 +2869,16 @@
         <v>38530725</v>
       </c>
       <c r="Z23">
-        <v>10459806</v>
+        <v>38530725</v>
       </c>
       <c r="AA23">
-        <v>10459806</v>
+        <v>38530725</v>
       </c>
       <c r="AB23">
-        <v>10459806</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+        <v>38530725</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>120</v>
       </c>
@@ -2955,16 +2955,16 @@
         <v>10459806</v>
       </c>
       <c r="Z24">
-        <v>19963581</v>
+        <v>10459806</v>
       </c>
       <c r="AA24">
-        <v>19963581</v>
+        <v>10459806</v>
       </c>
       <c r="AB24">
-        <v>19963581</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+        <v>10459806</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>121</v>
       </c>
@@ -3041,16 +3041,16 @@
         <v>19963581</v>
       </c>
       <c r="Z25">
-        <v>9982048.0773335192</v>
+        <v>19963581</v>
       </c>
       <c r="AA25">
-        <v>10081868.558106899</v>
+        <v>19963581</v>
       </c>
       <c r="AB25">
-        <v>10182687.2436879</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+        <v>19963581</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>122</v>
       </c>
@@ -3127,16 +3127,16 @@
         <v>9883215.9181520008</v>
       </c>
       <c r="Z26">
-        <v>2060484</v>
+        <v>9982048.0773335192</v>
       </c>
       <c r="AA26">
-        <v>2060484</v>
+        <v>10081868.558106899</v>
       </c>
       <c r="AB26">
-        <v>2060484</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+        <v>10182687.2436879</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>123</v>
       </c>
@@ -3213,16 +3213,16 @@
         <v>2060484</v>
       </c>
       <c r="Z27">
-        <v>5414095</v>
+        <v>2060484</v>
       </c>
       <c r="AA27">
-        <v>5414095</v>
+        <v>2060484</v>
       </c>
       <c r="AB27">
-        <v>5414095</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+        <v>2060484</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>124</v>
       </c>
@@ -3299,16 +3299,16 @@
         <v>5414095</v>
       </c>
       <c r="Z28">
-        <v>64097085</v>
+        <v>5414095</v>
       </c>
       <c r="AA28">
-        <v>64097085</v>
+        <v>5414095</v>
       </c>
       <c r="AB28">
-        <v>64097085</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+        <v>5414095</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>125</v>
       </c>
@@ -3385,16 +3385,16 @@
         <v>64097085</v>
       </c>
       <c r="Z29">
-        <v>328964937.54004401</v>
+        <v>64097085</v>
       </c>
       <c r="AA29">
-        <v>332254586.91544503</v>
+        <v>64097085</v>
       </c>
       <c r="AB29">
-        <v>335577132.78459901</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+        <v>64097085</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>126</v>
       </c>
@@ -3471,16 +3471,16 @@
         <v>325707858.95053899</v>
       </c>
       <c r="Z30">
-        <v>127338621</v>
+        <v>328964937.54004401</v>
       </c>
       <c r="AA30">
-        <v>127338621</v>
+        <v>332254586.91544503</v>
       </c>
       <c r="AB30">
-        <v>127338621</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+        <v>335577132.78459901</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>127</v>
       </c>
@@ -3557,16 +3557,16 @@
         <v>127338621</v>
       </c>
       <c r="Z31">
-        <v>1357380000</v>
+        <v>127338621</v>
       </c>
       <c r="AA31">
-        <v>1357380000</v>
+        <v>127338621</v>
       </c>
       <c r="AB31">
-        <v>1357380000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+        <v>127338621</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>128</v>
       </c>
@@ -3643,16 +3643,16 @@
         <v>1357380000</v>
       </c>
       <c r="Z32">
-        <v>36585872.127199002</v>
+        <v>1357380000</v>
       </c>
       <c r="AA32">
-        <v>36951730.848471001</v>
+        <v>1357380000</v>
       </c>
       <c r="AB32">
-        <v>37321248.156955697</v>
-      </c>
-    </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+        <v>1357380000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>129</v>
       </c>
@@ -3729,16 +3729,16 @@
         <v>36223635.769504003</v>
       </c>
       <c r="Z33">
-        <v>50219669</v>
+        <v>36585872.127199002</v>
       </c>
       <c r="AA33">
-        <v>50219669</v>
+        <v>36951730.848471001</v>
       </c>
       <c r="AB33">
-        <v>50219669</v>
-      </c>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
+        <v>37321248.156955697</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>130</v>
       </c>
@@ -3815,16 +3815,16 @@
         <v>50219669</v>
       </c>
       <c r="Z34">
-        <v>208497422.60631901</v>
+        <v>50219669</v>
       </c>
       <c r="AA34">
-        <v>210582396.83238199</v>
+        <v>50219669</v>
       </c>
       <c r="AB34">
-        <v>212688220.800706</v>
-      </c>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
+        <v>50219669</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>131</v>
       </c>
@@ -3901,16 +3901,16 @@
         <v>206433091.68942499</v>
       </c>
       <c r="Z35">
-        <v>1302981484.6773801</v>
+        <v>208497422.60631901</v>
       </c>
       <c r="AA35">
-        <v>1316011299.5241499</v>
+        <v>210582396.83238199</v>
       </c>
       <c r="AB35">
-        <v>1329171412.5193999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
+        <v>212688220.800706</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>132</v>
       </c>
@@ -3987,16 +3987,16 @@
         <v>1290080677.8984001</v>
       </c>
       <c r="Z36">
-        <v>127299584.95231999</v>
+        <v>1302981484.6773801</v>
       </c>
       <c r="AA36">
-        <v>128572580.801843</v>
+        <v>1316011299.5241499</v>
       </c>
       <c r="AB36">
-        <v>129858306.609862</v>
-      </c>
-    </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
+        <v>1329171412.5193999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>133</v>
       </c>
@@ -4073,16 +4073,16 @@
         <v>126039193.022099</v>
       </c>
       <c r="Z37">
-        <v>143499861</v>
+        <v>127299584.95231999</v>
       </c>
       <c r="AA37">
-        <v>143499861</v>
+        <v>128572580.801843</v>
       </c>
       <c r="AB37">
-        <v>143499861</v>
-      </c>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
+        <v>129858306.609862</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>134</v>
       </c>
@@ -4159,16 +4159,16 @@
         <v>143499861</v>
       </c>
       <c r="Z38">
-        <v>24070107.294909</v>
+        <v>143499861</v>
       </c>
       <c r="AA38">
-        <v>24310808.367858101</v>
+        <v>143499861</v>
       </c>
       <c r="AB38">
-        <v>24553916.4515367</v>
-      </c>
-    </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
+        <v>143499861</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>135</v>
       </c>
@@ -4245,16 +4245,16 @@
         <v>23831789.400899999</v>
       </c>
       <c r="Z39">
-        <v>8409622.5759428199</v>
+        <v>24070107.294909</v>
       </c>
       <c r="AA39">
-        <v>8493718.8017022498</v>
+        <v>24310808.367858101</v>
       </c>
       <c r="AB39">
-        <v>8578655.9897192698</v>
-      </c>
-    </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
+        <v>24553916.4515367</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>136</v>
       </c>
@@ -4331,16 +4331,16 @@
         <v>8326358.9860819997</v>
       </c>
       <c r="Z40">
-        <v>77975206.704490393</v>
+        <v>8409622.5759428199</v>
       </c>
       <c r="AA40">
-        <v>78754958.771535307</v>
+        <v>8493718.8017022498</v>
       </c>
       <c r="AB40">
-        <v>79542508.359250695</v>
-      </c>
-    </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+        <v>8578655.9897192698</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>137</v>
       </c>
@@ -4417,16 +4417,16 @@
         <v>77203174.954941005</v>
       </c>
       <c r="Z41">
-        <v>24548200</v>
+        <v>77975206.704490393</v>
       </c>
       <c r="AA41">
-        <v>24671800</v>
+        <v>78754958.771535307</v>
       </c>
       <c r="AB41">
-        <v>24795400</v>
-      </c>
-    </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+        <v>79542508.359250695</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>138</v>
       </c>
@@ -4503,16 +4503,16 @@
         <v>24424600</v>
       </c>
       <c r="Z42">
-        <v>5290628.5016019</v>
+        <v>24548200</v>
       </c>
       <c r="AA42">
-        <v>5343534.7866179198</v>
+        <v>24671800</v>
       </c>
       <c r="AB42">
-        <v>5396970.1344841002</v>
-      </c>
-    </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+        <v>24795400</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>139</v>
       </c>
@@ -4589,16 +4589,16 @@
         <v>5238246.0411900003</v>
       </c>
       <c r="Z43">
-        <v>260011177.57978001</v>
+        <v>5290628.5016019</v>
       </c>
       <c r="AA43">
-        <v>262611289.35557801</v>
+        <v>5343534.7866179198</v>
       </c>
       <c r="AB43">
-        <v>265237402.249134</v>
-      </c>
-    </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
+        <v>5396970.1344841002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>140</v>
       </c>
@@ -4675,16 +4675,16 @@
         <v>257436809.48493099</v>
       </c>
       <c r="Z44">
-        <v>52981991</v>
+        <v>260011177.57978001</v>
       </c>
       <c r="AA44">
-        <v>52981991</v>
+        <v>262611289.35557801</v>
       </c>
       <c r="AB44">
-        <v>52981991</v>
-      </c>
-    </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
+        <v>265237402.249134</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>141</v>
       </c>
@@ -4761,16 +4761,16 @@
         <v>52981991</v>
       </c>
       <c r="Z45">
-        <v>946083057.64657295</v>
+        <v>52981991</v>
       </c>
       <c r="AA45">
-        <v>958136077.71503901</v>
+        <v>52981991</v>
       </c>
       <c r="AB45">
-        <v>970382074.74282897</v>
-      </c>
-    </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
+        <v>52981991</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>142</v>
       </c>
@@ -4847,16 +4847,16 @@
         <v>934219697.41439104</v>
       </c>
       <c r="Z46">
-        <v>305555967.23308301</v>
+        <v>946083057.64657295</v>
       </c>
       <c r="AA46">
-        <v>308822200.968382</v>
+        <v>958136077.71503901</v>
       </c>
       <c r="AB46">
-        <v>312130095.143493</v>
-      </c>
-    </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
+        <v>970382074.74282897</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>143</v>
       </c>
@@ -4933,16 +4933,16 @@
         <v>302330806.771478</v>
       </c>
       <c r="Z47">
-        <v>75320157.828319401</v>
+        <v>305555967.23308301</v>
       </c>
       <c r="AA47">
-        <v>74743540.015641004</v>
+        <v>308822200.968382</v>
       </c>
       <c r="AB47">
-        <v>74173774.140445396</v>
-      </c>
-    </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
+        <v>312130095.143493</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>144</v>
       </c>
@@ -5019,16 +5019,16 @@
         <v>75903685.931290999</v>
       </c>
       <c r="Z48">
-        <v>1115948555.6883299</v>
+        <v>75320157.828319401</v>
       </c>
       <c r="AA48">
-        <v>1143298941.5368099</v>
+        <v>74743540.015641004</v>
       </c>
       <c r="AB48">
-        <v>1171375379.87463</v>
-      </c>
-    </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.3">
+        <v>74173774.140445396</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>145</v>
       </c>
@@ -5105,16 +5105,16 @@
         <v>1089304502.43628</v>
       </c>
       <c r="Z49">
-        <v>308588825.22870201</v>
+        <v>1115948555.6883299</v>
       </c>
       <c r="AA49">
-        <v>312903692.02448499</v>
+        <v>1143298941.5368099</v>
       </c>
       <c r="AB49">
-        <v>317296389.68719</v>
-      </c>
-    </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
+        <v>1171375379.87463</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>146</v>
       </c>
@@ -5189,6 +5189,15 @@
       </c>
       <c r="Y50">
         <v>304350158.01242101</v>
+      </c>
+      <c r="Z50">
+        <v>308588825.22870201</v>
+      </c>
+      <c r="AA50">
+        <v>312903692.02448499</v>
+      </c>
+      <c r="AB50">
+        <v>317296389.68719</v>
       </c>
     </row>
   </sheetData>
@@ -5201,13 +5210,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{439E3D99-3370-421D-978A-3B89B42E46AB}">
   <dimension ref="A1:AB50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>147</v>
       </c>
@@ -5284,7 +5293,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -5370,7 +5379,7 @@
         <v>397566.22750170197</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -5456,7 +5465,7 @@
         <v>476192.45719920401</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -5542,7 +5551,7 @@
         <v>60674.916851239999</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -5628,7 +5637,7 @@
         <v>21943.100360279801</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -5714,7 +5723,7 @@
         <v>223921.84415332499</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -5800,7 +5809,7 @@
         <v>3448971.4676544899</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -5886,7 +5895,7 @@
         <v>312732.76253566297</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -5972,7 +5981,7 @@
         <v>28111.746901512299</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -6058,7 +6067,7 @@
         <v>1244743.65745211</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>107</v>
       </c>
@@ -6144,7 +6153,7 @@
         <v>240550.522715848</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -6230,7 +6239,7 @@
         <v>2425652.7684032498</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -6316,7 +6325,7 @@
         <v>183409.320808841</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>110</v>
       </c>
@@ -6402,7 +6411,7 @@
         <v>53966.2115805258</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>111</v>
       </c>
@@ -6488,7 +6497,7 @@
         <v>146019.68992224699</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>112</v>
       </c>
@@ -6574,7 +6583,7 @@
         <v>356043.04297576699</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>113</v>
       </c>
@@ -6660,7 +6669,7 @@
         <v>1789706.24877002</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>114</v>
       </c>
@@ -6746,7 +6755,7 @@
         <v>48796.258919580599</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>115</v>
       </c>
@@ -6832,7 +6841,7 @@
         <v>63514.889779491699</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>116</v>
       </c>
@@ -6918,7 +6927,7 @@
         <v>30462.629372419298</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -7004,7 +7013,7 @@
         <v>13276.997685591399</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>118</v>
       </c>
@@ -7090,7 +7099,7 @@
         <v>810228.55126850901</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>119</v>
       </c>
@@ -7176,7 +7185,7 @@
         <v>532257.33535346994</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>120</v>
       </c>
@@ -7262,7 +7271,7 @@
         <v>213296.19029119</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>121</v>
       </c>
@@ -7348,7 +7357,7 @@
         <v>223381.83901910801</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>122</v>
       </c>
@@ -7434,7 +7443,7 @@
         <v>474215.15766411502</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>123</v>
       </c>
@@ -7520,7 +7529,7 @@
         <v>48391.4491370131</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>124</v>
       </c>
@@ -7606,7 +7615,7 @@
         <v>93863.039758582396</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>125</v>
       </c>
@@ -7692,7 +7701,7 @@
         <v>2524735.8563085799</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>126</v>
       </c>
@@ -7778,7 +7787,7 @@
         <v>19145355.962483201</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>127</v>
       </c>
@@ -7864,7 +7873,7 @@
         <v>4539942.6627166504</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>128</v>
       </c>
@@ -7950,7 +7959,7 @@
         <v>12811910.6428588</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>129</v>
       </c>
@@ -8036,7 +8045,7 @@
         <v>1555602.31311461</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>130</v>
       </c>
@@ -8122,7 +8131,7 @@
         <v>1470781.0895814099</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>131</v>
       </c>
@@ -8208,7 +8217,7 @@
         <v>1650554.57546281</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>132</v>
       </c>
@@ -8294,7 +8303,7 @@
         <v>2582923.0467437301</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>133</v>
       </c>
@@ -8380,7 +8389,7 @@
         <v>1122323.27846996</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>134</v>
       </c>
@@ -8466,7 +8475,7 @@
         <v>1512219.8761064401</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>135</v>
       </c>
@@ -8552,7 +8561,7 @@
         <v>1232878.81455894</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>136</v>
       </c>
@@ -8638,7 +8647,7 @@
         <v>653350.13056848105</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>137</v>
       </c>
@@ -8724,7 +8733,7 @@
         <v>680147.91621865903</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>138</v>
       </c>
@@ -8810,7 +8819,7 @@
         <v>491104.42155903199</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>139</v>
       </c>
@@ -8896,7 +8905,7 @@
         <v>360282.59369036398</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>140</v>
       </c>
@@ -8982,7 +8991,7 @@
         <v>999723.79086552805</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>141</v>
       </c>
@@ -9068,7 +9077,7 @@
         <v>313917.81258007302</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>142</v>
       </c>
@@ -9154,7 +9163,7 @@
         <v>3450302.7362932502</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>143</v>
       </c>
@@ -9240,7 +9249,7 @@
         <v>2108426.4138096799</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>144</v>
       </c>
@@ -9326,7 +9335,7 @@
         <v>346955.98255298502</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>145</v>
       </c>
@@ -9412,7 +9421,7 @@
         <v>1578465.6720205999</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>146</v>
       </c>

</xml_diff>